<commit_message>
some changes to transport technologies, added modalsplit for Road|RE for 2025; small fixes in BaseYearProduction and ResidualCapacity
</commit_message>
<xml_diff>
--- a/Data/Parameters/Par_CapitalCost/transport.xlsx
+++ b/Data/Parameters/Par_CapitalCost/transport.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28429"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28623"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\testbed\Documents\GENeSYS_MOD.data\Data\Parameters\Par_CapitalCost\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nim\Documents\GENeSYS_MOD.data\Data\Parameters\Par_CapitalCost\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C6034D14-DAC4-4EE2-B737-0D0B1A633B83}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5160483B-A424-4C12-80A8-D1992BAB988E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="30960" windowHeight="16800" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="costs" sheetId="2" r:id="rId1"/>
@@ -765,7 +765,7 @@
   <dimension ref="A1:AA32"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="R24" sqref="R24"/>
+      <selection activeCell="N26" sqref="N26:S27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1100,7 +1100,7 @@
         <v>165754</v>
       </c>
       <c r="D5">
-        <f t="shared" ref="D5:F23" si="15">(C5+E5)/2</f>
+        <f t="shared" ref="D5:F20" si="15">(C5+E5)/2</f>
         <v>165754</v>
       </c>
       <c r="E5" s="2">
@@ -1424,7 +1424,7 @@
         <v>391.85489999999999</v>
       </c>
       <c r="O8" s="3">
-        <f t="shared" si="24"/>
+        <f>ROUND((F8/($J8*$K8))*1000,4)</f>
         <v>391.85489999999999</v>
       </c>
       <c r="P8" s="3">
@@ -2027,7 +2027,7 @@
         <v>363.21717862992807</v>
       </c>
       <c r="S15" s="5">
-        <f t="shared" ref="S15:S24" si="30">0.05*L15</f>
+        <f t="shared" ref="S15:S19" si="30">0.05*L15</f>
         <v>19.759014517468088</v>
       </c>
       <c r="T15" s="5">
@@ -2035,23 +2035,23 @@
         <v>19.759014517468088</v>
       </c>
       <c r="U15" s="5">
-        <f t="shared" ref="U15:U24" si="31">0.05*M15</f>
+        <f t="shared" ref="U15:U19" si="31">0.05*M15</f>
         <v>18.959936724482244</v>
       </c>
       <c r="V15" s="5">
-        <f t="shared" ref="V15:V24" si="32">0.05*N15</f>
+        <f t="shared" ref="V15:V19" si="32">0.05*N15</f>
         <v>18.160858931496403</v>
       </c>
       <c r="W15" s="5">
-        <f t="shared" ref="W15:W24" si="33">0.05*O15</f>
+        <f t="shared" ref="W15:W19" si="33">0.05*O15</f>
         <v>18.160858931496403</v>
       </c>
       <c r="X15" s="5">
-        <f t="shared" ref="X15:X24" si="34">0.05*P15</f>
+        <f t="shared" ref="X15:X19" si="34">0.05*P15</f>
         <v>18.160858931496403</v>
       </c>
       <c r="Y15" s="5">
-        <f t="shared" ref="Y15:Y24" si="35">0.05*Q15</f>
+        <f t="shared" ref="Y15:Y19" si="35">0.05*Q15</f>
         <v>18.160858931496403</v>
       </c>
       <c r="AA15" t="s">
@@ -2124,7 +2124,7 @@
         <v>19.759014517468088</v>
       </c>
       <c r="T16" s="5">
-        <f t="shared" ref="T16:T24" si="43">0.05*L16</f>
+        <f t="shared" ref="T16:T19" si="43">0.05*L16</f>
         <v>19.759014517468088</v>
       </c>
       <c r="U16" s="5">
@@ -2452,25 +2452,25 @@
       </c>
       <c r="D20">
         <f t="shared" si="15"/>
-        <v>23337</v>
+        <v>22427</v>
       </c>
       <c r="E20">
-        <v>18110</v>
+        <v>16290</v>
       </c>
       <c r="F20">
         <f>E20-($E20-$I20)/4</f>
-        <v>17292.5</v>
+        <v>15705</v>
       </c>
       <c r="G20">
         <f t="shared" ref="G20:H20" si="46">F20-($E20-$I20)/4</f>
-        <v>16475</v>
+        <v>15120</v>
       </c>
       <c r="H20">
         <f t="shared" si="46"/>
-        <v>15657.5</v>
+        <v>14535</v>
       </c>
       <c r="I20">
-        <v>14840</v>
+        <v>13950</v>
       </c>
       <c r="J20">
         <v>1.6</v>
@@ -2484,27 +2484,27 @@
       </c>
       <c r="M20" s="3">
         <f t="shared" ref="M20:R20" si="47">ROUND((D20/($J20*$K20))*(1/1000000)*1000000000,4)</f>
-        <v>1080.4167</v>
+        <v>1038.287</v>
       </c>
       <c r="N20" s="3">
         <f t="shared" si="47"/>
-        <v>838.42589999999996</v>
+        <v>754.16669999999999</v>
       </c>
       <c r="O20" s="3">
         <f t="shared" si="47"/>
-        <v>800.57870000000003</v>
+        <v>727.08330000000001</v>
       </c>
       <c r="P20" s="3">
         <f t="shared" si="47"/>
-        <v>762.73149999999998</v>
+        <v>700</v>
       </c>
       <c r="Q20" s="3">
         <f t="shared" si="47"/>
-        <v>724.88430000000005</v>
+        <v>672.91669999999999</v>
       </c>
       <c r="R20" s="3">
         <f t="shared" si="47"/>
-        <v>687.03700000000003</v>
+        <v>645.83330000000001</v>
       </c>
       <c r="S20" s="5">
         <f>ROUND(0.05*L20,4)</f>
@@ -2512,27 +2512,27 @@
       </c>
       <c r="T20" s="5">
         <f t="shared" ref="T20:Y20" si="48">ROUND(0.05*M20,4)</f>
-        <v>54.020800000000001</v>
+        <v>51.914400000000001</v>
       </c>
       <c r="U20" s="5">
         <f t="shared" si="48"/>
-        <v>41.921300000000002</v>
+        <v>37.708300000000001</v>
       </c>
       <c r="V20" s="5">
         <f t="shared" si="48"/>
-        <v>40.0289</v>
+        <v>36.354199999999999</v>
       </c>
       <c r="W20" s="5">
         <f t="shared" si="48"/>
-        <v>38.136600000000001</v>
+        <v>35</v>
       </c>
       <c r="X20" s="5">
         <f t="shared" si="48"/>
-        <v>36.244199999999999</v>
+        <v>33.645800000000001</v>
       </c>
       <c r="Y20" s="5">
         <f t="shared" si="48"/>
-        <v>34.351900000000001</v>
+        <v>32.291699999999999</v>
       </c>
       <c r="Z20" t="s">
         <v>100</v>
@@ -2659,7 +2659,7 @@
         <v>17930</v>
       </c>
       <c r="G22">
-        <f t="shared" ref="F22:H22" si="64">F22-($E22-$I22)/4</f>
+        <f t="shared" ref="G22:H22" si="64">F22-($E22-$I22)/4</f>
         <v>17930</v>
       </c>
       <c r="H22">
@@ -2972,7 +2972,7 @@
       <c r="B32" t="s">
         <v>93</v>
       </c>
-      <c r="C32" s="2" t="s">
+      <c r="C32" s="4" t="s">
         <v>98</v>
       </c>
     </row>
@@ -2998,9 +2998,10 @@
   </dataValidations>
   <hyperlinks>
     <hyperlink ref="C28" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="C32" r:id="rId2" xr:uid="{ED75C4C0-A6AB-4635-AE39-AA72C13D6F13}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.78749999999999998" bottom="0.78749999999999998" header="0.511811023622047" footer="0.511811023622047"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId3"/>
 </worksheet>
 </file>
 

</xml_diff>